<commit_message>
changes in gitignore file
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/chooseTestEnvironment.xlsx
+++ b/src/test/resources/testData/chooseTestEnvironment.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pankaj.yadav\eclipse-workspace\ExposureHubEverest\src\test\resources\testData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pankaj.yadav\eclipse-workspace\ExposureHub\src\test\resources\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -380,7 +380,7 @@
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
changes in element to be clickable
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/chooseTestEnvironment.xlsx
+++ b/src/test/resources/testData/chooseTestEnvironment.xlsx
@@ -29,7 +29,7 @@
     <t>chooseTestEnvironment</t>
   </si>
   <si>
-    <t>Test</t>
+    <t>Test V2</t>
   </si>
 </sst>
 </file>
@@ -380,7 +380,7 @@
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
changes in edit schedule
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/chooseTestEnvironment.xlsx
+++ b/src/test/resources/testData/chooseTestEnvironment.xlsx
@@ -29,7 +29,7 @@
     <t>chooseTestEnvironment</t>
   </si>
   <si>
-    <t>Test V2</t>
+    <t>Test</t>
   </si>
 </sst>
 </file>
@@ -380,7 +380,7 @@
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
changes in report to add project logo
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/chooseTestEnvironment.xlsx
+++ b/src/test/resources/testData/chooseTestEnvironment.xlsx
@@ -380,7 +380,7 @@
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -401,7 +401,7 @@
   </sheetData>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2">
-      <formula1>"Test,Test V2,Oilfield"</formula1>
+      <formula1>"Test,Test V2"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>